<commit_message>
Excel is working fine now
</commit_message>
<xml_diff>
--- a/MeetingRoomData.xlsx
+++ b/MeetingRoomData.xlsx
@@ -7,165 +7,165 @@
     <workbookView xWindow="120" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="15-04-2018" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Template" sheetId="6" r:id="rId1"/>
+    <sheet name="26-04-2018" sheetId="5" r:id="rId2"/>
+    <sheet name="15-04-2018" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="50">
+  <si>
+    <t>Booked On</t>
+  </si>
+  <si>
+    <t>Slot 1</t>
+  </si>
+  <si>
+    <t>Slot 2</t>
+  </si>
+  <si>
+    <t>Slot 3</t>
+  </si>
+  <si>
+    <t>Slot 4</t>
+  </si>
+  <si>
+    <t>Slot 5</t>
+  </si>
+  <si>
+    <t>Slot 6</t>
+  </si>
+  <si>
+    <t>Slot 7</t>
+  </si>
+  <si>
+    <t>Slot 8</t>
+  </si>
+  <si>
+    <t>Slot 9</t>
+  </si>
+  <si>
+    <t>Slot 10</t>
+  </si>
+  <si>
+    <t>Slot 11</t>
+  </si>
+  <si>
+    <t>Slot 12</t>
+  </si>
+  <si>
+    <t>Slot 13</t>
+  </si>
+  <si>
+    <t>Slot 14</t>
+  </si>
+  <si>
+    <t>Slot 15</t>
+  </si>
+  <si>
+    <t>Slot 16</t>
+  </si>
+  <si>
+    <t>Slot 17</t>
+  </si>
+  <si>
+    <t>Slot 18</t>
+  </si>
+  <si>
+    <t>Slot 19</t>
+  </si>
+  <si>
+    <t>Slot 20</t>
+  </si>
+  <si>
+    <t>Slot 21</t>
+  </si>
+  <si>
+    <t>Slot 22</t>
+  </si>
+  <si>
+    <t>Slot 23</t>
+  </si>
+  <si>
+    <t>Slot 24</t>
+  </si>
+  <si>
+    <t>Slot 25</t>
+  </si>
+  <si>
+    <t>Slot 26</t>
+  </si>
+  <si>
+    <t>Slot 27</t>
+  </si>
+  <si>
+    <t>Slot 28</t>
+  </si>
+  <si>
+    <t>Slot 29</t>
+  </si>
+  <si>
+    <t>Slot 30</t>
+  </si>
+  <si>
+    <t>Slot 31</t>
+  </si>
+  <si>
+    <t>Slot 32</t>
+  </si>
+  <si>
+    <t>Slot 33</t>
+  </si>
+  <si>
+    <t>Slot 34</t>
+  </si>
+  <si>
+    <t>Slot 35</t>
+  </si>
+  <si>
+    <t>Slot 36</t>
+  </si>
+  <si>
+    <t>Slot 37</t>
+  </si>
+  <si>
+    <t>Slot 38</t>
+  </si>
+  <si>
+    <t>Slot 39</t>
+  </si>
+  <si>
+    <t>Slot 40</t>
+  </si>
+  <si>
+    <t>Slot 41</t>
+  </si>
+  <si>
+    <t>Slot 42</t>
+  </si>
+  <si>
+    <t>Slot 43</t>
+  </si>
+  <si>
+    <t>Slot 44</t>
+  </si>
+  <si>
+    <t>Slot 45</t>
+  </si>
+  <si>
+    <t>Slot 46</t>
+  </si>
+  <si>
+    <t>Slot 47</t>
+  </si>
+  <si>
+    <t>Slot 48</t>
+  </si>
   <si>
     <t>Room #</t>
-  </si>
-  <si>
-    <t>Booked On</t>
-  </si>
-  <si>
-    <t>Slot 1</t>
-  </si>
-  <si>
-    <t>Slot 2</t>
-  </si>
-  <si>
-    <t>Slot 3</t>
-  </si>
-  <si>
-    <t>Slot 4</t>
-  </si>
-  <si>
-    <t>Slot 5</t>
-  </si>
-  <si>
-    <t>Slot 6</t>
-  </si>
-  <si>
-    <t>Slot 7</t>
-  </si>
-  <si>
-    <t>Slot 8</t>
-  </si>
-  <si>
-    <t>Slot 9</t>
-  </si>
-  <si>
-    <t>Slot 10</t>
-  </si>
-  <si>
-    <t>Slot 11</t>
-  </si>
-  <si>
-    <t>Slot 12</t>
-  </si>
-  <si>
-    <t>Slot 13</t>
-  </si>
-  <si>
-    <t>Slot 14</t>
-  </si>
-  <si>
-    <t>Slot 15</t>
-  </si>
-  <si>
-    <t>Slot 16</t>
-  </si>
-  <si>
-    <t>Slot 17</t>
-  </si>
-  <si>
-    <t>Slot 18</t>
-  </si>
-  <si>
-    <t>Slot 19</t>
-  </si>
-  <si>
-    <t>Slot 20</t>
-  </si>
-  <si>
-    <t>Slot 21</t>
-  </si>
-  <si>
-    <t>Slot 22</t>
-  </si>
-  <si>
-    <t>Slot 23</t>
-  </si>
-  <si>
-    <t>Slot 24</t>
-  </si>
-  <si>
-    <t>Slot 25</t>
-  </si>
-  <si>
-    <t>Slot 26</t>
-  </si>
-  <si>
-    <t>Slot 27</t>
-  </si>
-  <si>
-    <t>Slot 28</t>
-  </si>
-  <si>
-    <t>Slot 29</t>
-  </si>
-  <si>
-    <t>Slot 30</t>
-  </si>
-  <si>
-    <t>Slot 31</t>
-  </si>
-  <si>
-    <t>Slot 32</t>
-  </si>
-  <si>
-    <t>Slot 33</t>
-  </si>
-  <si>
-    <t>Slot 34</t>
-  </si>
-  <si>
-    <t>Slot 35</t>
-  </si>
-  <si>
-    <t>Slot 36</t>
-  </si>
-  <si>
-    <t>Slot 37</t>
-  </si>
-  <si>
-    <t>Slot 38</t>
-  </si>
-  <si>
-    <t>Slot 39</t>
-  </si>
-  <si>
-    <t>Slot 40</t>
-  </si>
-  <si>
-    <t>Slot 41</t>
-  </si>
-  <si>
-    <t>Slot 42</t>
-  </si>
-  <si>
-    <t>Slot 43</t>
-  </si>
-  <si>
-    <t>Slot 44</t>
-  </si>
-  <si>
-    <t>Slot 45</t>
-  </si>
-  <si>
-    <t>Slot 46</t>
-  </si>
-  <si>
-    <t>Slot 47</t>
-  </si>
-  <si>
-    <t>Slot 48</t>
   </si>
 </sst>
 </file>
@@ -173,7 +173,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -206,7 +206,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,7 +511,473 @@
   <dimension ref="A1:AX11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="50" width="6.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AX11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="50" width="6.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AX11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,161 +990,158 @@
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>48</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="C2">
         <v>1</v>
       </c>
     </row>
@@ -731,28 +1194,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Reading and populating the meetingRoomList done
</commit_message>
<xml_diff>
--- a/MeetingRoomData.xlsx
+++ b/MeetingRoomData.xlsx
@@ -4,22 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="6" r:id="rId1"/>
     <sheet name="26-04-2018" sheetId="5" r:id="rId2"/>
-    <sheet name="15-04-2018" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="50">
-  <si>
-    <t>Booked On</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
   <si>
     <t>Slot 1</t>
   </si>
@@ -172,9 +168,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -204,9 +197,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,25 +500,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX11"/>
+  <dimension ref="A1:AW11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="W1" workbookViewId="0">
+      <selection sqref="A1:AW11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="50" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="50" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
@@ -670,69 +661,56 @@
       <c r="AW1" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -741,25 +719,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX11"/>
+  <dimension ref="A1:AW11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="50" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="50" width="6.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
@@ -903,295 +880,148 @@
       <c r="AW1" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="50" width="6.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Made logical Changes to make the UI better for UX
</commit_message>
<xml_diff>
--- a/MeetingRoomData.xlsx
+++ b/MeetingRoomData.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="6" r:id="rId1"/>
-    <sheet name="26-04-2018" sheetId="5" r:id="rId2"/>
+    <sheet name="Template" sheetId="10" r:id="rId1"/>
+    <sheet name="27-04-2018" sheetId="9" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="59">
   <si>
     <t>Slot 1</t>
   </si>
@@ -162,6 +162,36 @@
   </si>
   <si>
     <t>Room #</t>
+  </si>
+  <si>
+    <t>MR1</t>
+  </si>
+  <si>
+    <t>MR2</t>
+  </si>
+  <si>
+    <t>MR3</t>
+  </si>
+  <si>
+    <t>MR4</t>
+  </si>
+  <si>
+    <t>MR5</t>
+  </si>
+  <si>
+    <t>MR6</t>
+  </si>
+  <si>
+    <t>MR7</t>
+  </si>
+  <si>
+    <t>MR8</t>
+  </si>
+  <si>
+    <t>MR9</t>
+  </si>
+  <si>
+    <t>MR10</t>
   </si>
 </sst>
 </file>
@@ -502,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW11"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection sqref="A1:AW11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,53 +693,1493 @@
       </c>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+      <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3">
+        <v>0</v>
+      </c>
+      <c r="AW3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>0</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6">
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>0</v>
+      </c>
+      <c r="AV6">
+        <v>0</v>
+      </c>
+      <c r="AW6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
+      <c r="AT7">
+        <v>0</v>
+      </c>
+      <c r="AU7">
+        <v>0</v>
+      </c>
+      <c r="AV7">
+        <v>0</v>
+      </c>
+      <c r="AW7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>0</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>0</v>
+      </c>
+      <c r="AU8">
+        <v>0</v>
+      </c>
+      <c r="AV8">
+        <v>0</v>
+      </c>
+      <c r="AW8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>0</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>0</v>
+      </c>
+      <c r="AS9">
+        <v>0</v>
+      </c>
+      <c r="AT9">
+        <v>0</v>
+      </c>
+      <c r="AU9">
+        <v>0</v>
+      </c>
+      <c r="AV9">
+        <v>0</v>
+      </c>
+      <c r="AW9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>0</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10">
+        <v>0</v>
+      </c>
+      <c r="AO10">
+        <v>0</v>
+      </c>
+      <c r="AP10">
+        <v>0</v>
+      </c>
+      <c r="AQ10">
+        <v>0</v>
+      </c>
+      <c r="AR10">
+        <v>0</v>
+      </c>
+      <c r="AS10">
+        <v>0</v>
+      </c>
+      <c r="AT10">
+        <v>0</v>
+      </c>
+      <c r="AU10">
+        <v>0</v>
+      </c>
+      <c r="AV10">
+        <v>0</v>
+      </c>
+      <c r="AW10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AK11">
+        <v>0</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
+      </c>
+      <c r="AM11">
+        <v>0</v>
+      </c>
+      <c r="AN11">
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>0</v>
+      </c>
+      <c r="AP11">
+        <v>0</v>
+      </c>
+      <c r="AQ11">
+        <v>0</v>
+      </c>
+      <c r="AR11">
+        <v>0</v>
+      </c>
+      <c r="AS11">
+        <v>0</v>
+      </c>
+      <c r="AT11">
+        <v>0</v>
+      </c>
+      <c r="AU11">
+        <v>0</v>
+      </c>
+      <c r="AV11">
+        <v>0</v>
+      </c>
+      <c r="AW11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -721,8 +2191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,8 +2352,8 @@
       </c>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>49</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -892,12 +2362,147 @@
         <v>0</v>
       </c>
       <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>50</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -906,12 +2511,147 @@
         <v>0</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
+        <v>0</v>
+      </c>
+      <c r="AS3">
+        <v>0</v>
+      </c>
+      <c r="AT3">
+        <v>0</v>
+      </c>
+      <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3">
+        <v>0</v>
+      </c>
+      <c r="AW3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>51</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -920,12 +2660,147 @@
         <v>0</v>
       </c>
       <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>0</v>
+      </c>
+      <c r="AI4">
+        <v>0</v>
+      </c>
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
+        <v>0</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>0</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4">
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>0</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>52</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -934,12 +2809,147 @@
         <v>0</v>
       </c>
       <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
+        <v>0</v>
+      </c>
+      <c r="AS5">
+        <v>0</v>
+      </c>
+      <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>53</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -948,12 +2958,147 @@
         <v>0</v>
       </c>
       <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6">
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>0</v>
+      </c>
+      <c r="AV6">
+        <v>0</v>
+      </c>
+      <c r="AW6">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
+      <c r="A7" t="s">
+        <v>54</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -962,12 +3107,147 @@
         <v>0</v>
       </c>
       <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+      <c r="AH7">
+        <v>0</v>
+      </c>
+      <c r="AI7">
+        <v>0</v>
+      </c>
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
+        <v>0</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
+        <v>0</v>
+      </c>
+      <c r="AT7">
+        <v>0</v>
+      </c>
+      <c r="AU7">
+        <v>0</v>
+      </c>
+      <c r="AV7">
+        <v>0</v>
+      </c>
+      <c r="AW7">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
+      <c r="A8" t="s">
+        <v>55</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -976,12 +3256,147 @@
         <v>0</v>
       </c>
       <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>0</v>
+      </c>
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>0</v>
+      </c>
+      <c r="AO8">
+        <v>0</v>
+      </c>
+      <c r="AP8">
+        <v>0</v>
+      </c>
+      <c r="AQ8">
+        <v>0</v>
+      </c>
+      <c r="AR8">
+        <v>0</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8">
+        <v>0</v>
+      </c>
+      <c r="AU8">
+        <v>0</v>
+      </c>
+      <c r="AV8">
+        <v>0</v>
+      </c>
+      <c r="AW8">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
+      <c r="A9" t="s">
+        <v>56</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -990,12 +3405,147 @@
         <v>0</v>
       </c>
       <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
+        <v>0</v>
+      </c>
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>0</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>0</v>
+      </c>
+      <c r="AS9">
+        <v>0</v>
+      </c>
+      <c r="AT9">
+        <v>0</v>
+      </c>
+      <c r="AU9">
+        <v>0</v>
+      </c>
+      <c r="AV9">
+        <v>0</v>
+      </c>
+      <c r="AW9">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
+      <c r="A10" t="s">
+        <v>57</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1004,12 +3554,147 @@
         <v>0</v>
       </c>
       <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <v>0</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>0</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10">
+        <v>0</v>
+      </c>
+      <c r="AO10">
+        <v>0</v>
+      </c>
+      <c r="AP10">
+        <v>0</v>
+      </c>
+      <c r="AQ10">
+        <v>0</v>
+      </c>
+      <c r="AR10">
+        <v>0</v>
+      </c>
+      <c r="AS10">
+        <v>0</v>
+      </c>
+      <c r="AT10">
+        <v>0</v>
+      </c>
+      <c r="AU10">
+        <v>0</v>
+      </c>
+      <c r="AV10">
+        <v>0</v>
+      </c>
+      <c r="AW10">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
+      <c r="A11" t="s">
+        <v>58</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -1018,6 +3703,141 @@
         <v>0</v>
       </c>
       <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AK11">
+        <v>0</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
+      </c>
+      <c r="AM11">
+        <v>0</v>
+      </c>
+      <c r="AN11">
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>0</v>
+      </c>
+      <c r="AP11">
+        <v>0</v>
+      </c>
+      <c r="AQ11">
+        <v>0</v>
+      </c>
+      <c r="AR11">
+        <v>0</v>
+      </c>
+      <c r="AS11">
+        <v>0</v>
+      </c>
+      <c r="AT11">
+        <v>0</v>
+      </c>
+      <c r="AU11">
+        <v>0</v>
+      </c>
+      <c r="AV11">
+        <v>0</v>
+      </c>
+      <c r="AW11">
         <v>0</v>
       </c>
     </row>

</xml_diff>